<commit_message>
fix logfile, updat list
</commit_message>
<xml_diff>
--- a/LimitCheck.xlsx
+++ b/LimitCheck.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achims_tab\Documents\own_SW\stock_check\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vollmera\Documents\SVN_home\trunk\SW_app\github\stock_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10583F5E-CE39-4EEF-8A08-BB48A6F4BD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50B5194-FA00-4D46-BF27-8397196026DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Have_List" sheetId="1" r:id="rId1"/>
@@ -864,16 +864,16 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.06640625" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -905,7 +905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -931,7 +931,7 @@
         <v>44510</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -957,7 +957,7 @@
         <v>44265</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -983,7 +983,7 @@
         <v>44114</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>44387</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>44387</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>44265</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>43901</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -1633,15 +1633,15 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>116</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>118</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>119</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>120</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>121</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>122</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>147</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>151</v>
       </c>
@@ -2131,30 +2131,54 @@
         <v>5</v>
       </c>
       <c r="I41" s="5">
-        <v>44197</v>
+        <v>44202</v>
       </c>
       <c r="J41" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H42">
+        <v>5</v>
+      </c>
+      <c r="I42" s="5">
+        <v>44202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H43">
+        <v>5</v>
+      </c>
+      <c r="I43" s="5">
+        <v>44202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44" s="5">
+        <v>44202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>155</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="I45" s="5">
+        <v>44202</v>
       </c>
     </row>
   </sheetData>
@@ -2171,13 +2195,13 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2206,7 +2230,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -2217,7 +2241,7 @@
         <v>44075</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -2228,7 +2252,7 @@
         <v>44075</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -2239,7 +2263,7 @@
         <v>44075</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -2250,7 +2274,7 @@
         <v>44075</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
test for impoved log file
</commit_message>
<xml_diff>
--- a/LimitCheck.xlsx
+++ b/LimitCheck.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vollmera\Documents\SVN_home\trunk\SW_app\github\stock_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50B5194-FA00-4D46-BF27-8397196026DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3187BF26-615E-4871-AF71-D5D128341866}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Have_List" sheetId="1" r:id="rId1"/>
@@ -1632,7 +1632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B380F7C2-8FCD-4764-9E2D-3EDBCFAD427C}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
@@ -2191,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2246,7 +2246,7 @@
         <v>105</v>
       </c>
       <c r="H3">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="I3" s="5">
         <v>44075</v>
@@ -2257,7 +2257,7 @@
         <v>92</v>
       </c>
       <c r="H4">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I4" s="5">
         <v>44075</v>
@@ -2268,7 +2268,7 @@
         <v>106</v>
       </c>
       <c r="H5">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="I5" s="5">
         <v>44075</v>
@@ -2277,6 +2277,9 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
+      </c>
+      <c r="F6">
+        <v>10000</v>
       </c>
       <c r="H6">
         <v>40</v>

</xml_diff>

<commit_message>
runn all sheet, add peleton supervision
</commit_message>
<xml_diff>
--- a/LimitCheck.xlsx
+++ b/LimitCheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vollmera\Documents\SVN_home\trunk\SW_app\github\stock_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B600B0FB-0F01-4909-A3C8-D08E4482C26B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A910C0-AB6F-4059-A380-9912D6D52229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="157">
   <si>
     <t>WKN</t>
   </si>
@@ -1633,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B380F7C2-8FCD-4764-9E2D-3EDBCFAD427C}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2193,6 +2193,17 @@
       </c>
       <c r="I46" s="5">
         <v>44202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>115</v>
+      </c>
+      <c r="H47">
+        <v>8</v>
+      </c>
+      <c r="I47" s="5">
+        <v>44197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>